<commit_message>
save at 11:30 1/4/2024
</commit_message>
<xml_diff>
--- a/Source/dữ liệu/Book1.xlsx
+++ b/Source/dữ liệu/Book1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Wembley\Code_WEMBLEY\test_22-3-2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\khang\PDA\Wembley AR\May nut chan\Source\dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF6E5B9F-E657-4F6D-B443-52E363B00C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6D1B758-DE67-4A8A-9E56-CFD1052B70DC}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="315">
   <si>
     <t>Y0</t>
   </si>
@@ -753,13 +752,241 @@
   </si>
   <si>
     <t>Y5</t>
+  </si>
+  <si>
+    <t>S1 Horizontal P &amp; P Slide Forward</t>
+  </si>
+  <si>
+    <t>S1 Horizontal P &amp; P Slide Reverse</t>
+  </si>
+  <si>
+    <t>S1 Pick &amp; Place Gripper On</t>
+  </si>
+  <si>
+    <t>S1 Pick &amp; Place Gripper Off</t>
+  </si>
+  <si>
+    <t>S1 Singling Plate Vert Lifting Cyl Up</t>
+  </si>
+  <si>
+    <t>S1 Singling Plate Vert Lifting Cyl Dn</t>
+  </si>
+  <si>
+    <t>S2 Pick &amp; Place Vacuum On/Off</t>
+  </si>
+  <si>
+    <t>S2 Horizontal P &amp; P Cylinder Forward</t>
+  </si>
+  <si>
+    <t>S2 Air Blow On/Off</t>
+  </si>
+  <si>
+    <t>S2 Singling Plate Vert Lifting Cyl Dn</t>
+  </si>
+  <si>
+    <t>S2 Horizonal P &amp; P Cylinder Reverse</t>
+  </si>
+  <si>
+    <t>S2 Job Relieve Air Blow On/Off</t>
+  </si>
+  <si>
+    <t>S2 Singling Plate Vert Lifting Cyl Up</t>
+  </si>
+  <si>
+    <t>S2 Singling Plate Vacuum On/Off</t>
+  </si>
+  <si>
+    <t>S3 Job Holding Cylinder Forward</t>
+  </si>
+  <si>
+    <t>S3 Job Holding Cylinder Reverse</t>
+  </si>
+  <si>
+    <t>S5 Vertical Slide Up</t>
+  </si>
+  <si>
+    <t>S5 Vertical Slide Down</t>
+  </si>
+  <si>
+    <t>S12 Gripper On</t>
+  </si>
+  <si>
+    <t>S12 Gripper Off</t>
+  </si>
+  <si>
+    <t>S11 Horizontal P&amp;P Slide Forward</t>
+  </si>
+  <si>
+    <t>S11 Gripper On</t>
+  </si>
+  <si>
+    <t>S11 Gripper Off</t>
+  </si>
+  <si>
+    <t>S11 Horizontal P&amp;P Slide Reverse</t>
+  </si>
+  <si>
+    <t>S10 Holding Cylinder Fwd</t>
+  </si>
+  <si>
+    <t>S10 Holding Cylinder Rev</t>
+  </si>
+  <si>
+    <t>S6 Support Cylinder Up</t>
+  </si>
+  <si>
+    <t>S6 Support Cylinder Down</t>
+  </si>
+  <si>
+    <t>S6 Job Holding Cylinder Forward</t>
+  </si>
+  <si>
+    <t>S6 Job Holding Cylinder Reverse</t>
+  </si>
+  <si>
+    <t>S7 Weld Start</t>
+  </si>
+  <si>
+    <t>S7 Support Cylinder Up</t>
+  </si>
+  <si>
+    <t>S7 Support Cylinder Down</t>
+  </si>
+  <si>
+    <t>S4 Horizontal P &amp; P Slide Forward</t>
+  </si>
+  <si>
+    <t>S4 Horizontal P &amp; P Slide Reverse</t>
+  </si>
+  <si>
+    <t>S4 Singling Plate Vert Lifting Cyl Up</t>
+  </si>
+  <si>
+    <t>S1 Bowl Feeder Singling Vacuum TR1</t>
+  </si>
+  <si>
+    <t>S1 Bowl Feeder Singling Vacuum TR2</t>
+  </si>
+  <si>
+    <t>S1 Bowl Feeder Singling Vacuum TR3</t>
+  </si>
+  <si>
+    <t>S1 Bowl Feeder Singling Vacuum TR4</t>
+  </si>
+  <si>
+    <t>S2 Vacuum On/Off</t>
+  </si>
+  <si>
+    <t>S4 Bowl Feeder-2 On/Off</t>
+  </si>
+  <si>
+    <t>S1 Air Blow-1 On/Off</t>
+  </si>
+  <si>
+    <t>S1 Air Blow-2 On/Off</t>
+  </si>
+  <si>
+    <t>S4 Air Blow-1 On/Off</t>
+  </si>
+  <si>
+    <t>S4 Air Blow-2 On/Off</t>
+  </si>
+  <si>
+    <t>S2 Singling Vacuum-1 On/Off</t>
+  </si>
+  <si>
+    <t>S2 Singling Vacuum-2 On/Off</t>
+  </si>
+  <si>
+    <t>S10 Leak Test Air Blow On/Off Tr1</t>
+  </si>
+  <si>
+    <t>S10 Leak Test Air Blow On/Off Tr2</t>
+  </si>
+  <si>
+    <t>S10 Leak Test Air Blow On/Off Tr3</t>
+  </si>
+  <si>
+    <t>S10 Leak Test Air Blow On/Off Tr4</t>
+  </si>
+  <si>
+    <t>S2 Spare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6 Weld Start </t>
+  </si>
+  <si>
+    <t>S6 Weld Machine Reset</t>
+  </si>
+  <si>
+    <t>S6 Spare</t>
+  </si>
+  <si>
+    <t>S7 Weld Machine Reset</t>
+  </si>
+  <si>
+    <t>S7 Spare</t>
+  </si>
+  <si>
+    <t>S1 Conveyor Motor On/Off</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Up TR1</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Down TR1</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Up TR2</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Down TR2</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Up TR3</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Down TR3</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Up TR4</t>
+  </si>
+  <si>
+    <t>S3 Silicon Pressing Cylinder Down TR4</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-1 On</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-1 Off</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-2 On</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-2 Off</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-3 On</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-3 Off</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-4 On</t>
+  </si>
+  <si>
+    <t>S4 Pick &amp; Place Gripper-4 Off</t>
+  </si>
+  <si>
+    <t>S4 Singling Plate Vert Lifting Cyl Down</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,18 +995,51 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -809,10 +1069,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1148,982 +1418,1345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778F5B4E-91BC-4C33-BC73-5D879A7E0F44}">
-  <dimension ref="B3:P36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="4" width="26.5546875" customWidth="1"/>
-    <col min="7" max="8" width="33.33203125" customWidth="1"/>
-    <col min="11" max="12" width="25.77734375" customWidth="1"/>
-    <col min="15" max="16" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="7" max="8" width="33.375" customWidth="1"/>
+    <col min="11" max="11" width="25.75" customWidth="1"/>
+    <col min="12" max="12" width="29.125" customWidth="1"/>
+    <col min="15" max="15" width="26.625" customWidth="1"/>
+    <col min="16" max="16" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:16" ht="15.75">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="N3" s="1" t="s">
+      <c r="L3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="P3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="J4" s="1" t="s">
+      <c r="H4" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="N4" s="1" t="s">
+      <c r="L4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="P4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="15.75">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="F5" s="1" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="J5" s="1" t="s">
+      <c r="H5" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="N5" s="1" t="s">
+      <c r="L5" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="P5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="15.75">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="F6" s="1" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="1" t="s">
+      <c r="H6" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="N6" s="1" t="s">
+      <c r="L6" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="P6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="15.75">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="F7" s="1" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="J7" s="1" t="s">
+      <c r="H7" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="N7" s="1" t="s">
+      <c r="L7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="P7" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75">
+      <c r="B8" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="F8" s="1" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="J8" s="1" t="s">
+      <c r="H8" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="N8" s="1" t="s">
+      <c r="L8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="P8" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="F9" s="1" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="J9" s="1" t="s">
+      <c r="H9" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="N9" s="1" t="s">
+      <c r="L9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="P9" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="15.75">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="F10" s="1" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="J10" s="1" t="s">
+      <c r="H10" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="N10" s="1" t="s">
+      <c r="L10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="P10" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="15.75">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="F11" s="1" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="J11" s="1" t="s">
+      <c r="H11" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="N11" s="1" t="s">
+      <c r="L11" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+      <c r="P11" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="F12" s="1" t="s">
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="J12" s="1" t="s">
+      <c r="H12" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="N12" s="1" t="s">
+      <c r="L12" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="P12" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="15.75">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="F13" s="1" t="s">
+      <c r="D13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="N13" s="1" t="s">
+      <c r="L13" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+      <c r="P13" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15.75">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="F14" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="J14" s="1" t="s">
+      <c r="H14" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="N14" s="1" t="s">
+      <c r="L14" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="2:16" ht="15.75">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="F15" s="1" t="s">
+      <c r="D15" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="J15" s="1" t="s">
+      <c r="H15" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="N15" s="1" t="s">
+      <c r="L15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="2:16" ht="15.75">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="F16" s="1" t="s">
+      <c r="D16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" s="1" t="s">
+      <c r="H16" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="N16" s="1" t="s">
+      <c r="L16" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="2:16" ht="15.75">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="F17" s="1" t="s">
+      <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="J17" s="1" t="s">
+      <c r="H17" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="N17" s="1" t="s">
+      <c r="L17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="2:16" ht="15.75">
+      <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="F18" s="1" t="s">
+      <c r="D18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="J18" s="1" t="s">
+      <c r="H18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="N18" s="1" t="s">
+      <c r="L18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="2:16" ht="15">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" ht="15">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" ht="15.75">
+      <c r="B21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="F21" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="J21" s="1" t="s">
+      <c r="H21" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L21" s="2"/>
-      <c r="N21" s="1" t="s">
+      <c r="L21" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O21" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+      <c r="P21" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75">
+      <c r="B22" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="F22" s="1" t="s">
+      <c r="D22" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="J22" s="1" t="s">
+      <c r="H22" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="N22" s="1" t="s">
+      <c r="L22" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O22" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
+      <c r="P22" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.75">
+      <c r="B23" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="F23" s="1" t="s">
+      <c r="D23" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="J23" s="1" t="s">
+      <c r="H23" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="L23" s="2"/>
-      <c r="N23" s="1" t="s">
+      <c r="L23" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="O23" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+      <c r="P23" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="15.75">
+      <c r="B24" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="F24" s="1" t="s">
+      <c r="D24" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="J24" s="1" t="s">
+      <c r="H24" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="L24" s="2"/>
-      <c r="N24" s="1" t="s">
+      <c r="L24" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+      <c r="P24" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.75">
+      <c r="B25" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="F25" s="1" t="s">
+      <c r="D25" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="J25" s="1" t="s">
+      <c r="H25" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="L25" s="2"/>
-      <c r="N25" s="1" t="s">
+      <c r="L25" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="O25" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
+      <c r="P25" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.75">
+      <c r="B26" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="F26" s="1" t="s">
+      <c r="D26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="J26" s="1" t="s">
+      <c r="H26" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="L26" s="2"/>
-      <c r="N26" s="1" t="s">
+      <c r="L26" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O26" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="P26" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="15.75">
+      <c r="B27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="F27" s="1" t="s">
+      <c r="D27" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="J27" s="1" t="s">
+      <c r="H27" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="L27" s="2"/>
-      <c r="N27" s="1" t="s">
+      <c r="L27" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="O27" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+      <c r="P27" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15.75">
+      <c r="B28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="F28" s="1" t="s">
+      <c r="D28" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="J28" s="1" t="s">
+      <c r="H28" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="L28" s="2"/>
-      <c r="N28" s="1" t="s">
+      <c r="L28" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="O28" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+      <c r="P28" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15.75">
+      <c r="B29" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="F29" s="1" t="s">
+      <c r="D29" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="J29" s="1" t="s">
+      <c r="H29" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="L29" s="2"/>
-      <c r="N29" s="1" t="s">
+      <c r="L29" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="O29" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+      <c r="P29" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="15.75">
+      <c r="B30" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="F30" s="1" t="s">
+      <c r="D30" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="J30" s="1" t="s">
+      <c r="H30" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="L30" s="2"/>
-      <c r="N30" s="1" t="s">
+      <c r="L30" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="O30" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
+      <c r="P30" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="15.75">
+      <c r="B31" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="F31" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="J31" s="1" t="s">
+      <c r="H31" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="L31" s="2"/>
-      <c r="N31" s="1" t="s">
+      <c r="L31" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="O31" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
+      <c r="P31" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="15.75">
+      <c r="B32" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="F32" s="1" t="s">
+      <c r="D32" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="J32" s="1" t="s">
+      <c r="H32" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="L32" s="2"/>
-      <c r="N32" s="1" t="s">
+      <c r="L32" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="N32" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="O32" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="1" t="s">
+      <c r="P32" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" ht="15.75">
+      <c r="B33" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="F33" s="1" t="s">
+      <c r="D33" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="J33" s="1" t="s">
+      <c r="H33" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="K33" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="L33" s="2"/>
-      <c r="N33" s="1" t="s">
+      <c r="L33" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="M33" s="1"/>
+      <c r="N33" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="O33" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
+      <c r="P33" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="R33" s="4"/>
+    </row>
+    <row r="34" spans="2:18" ht="15.75">
+      <c r="B34" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="F34" s="1" t="s">
+      <c r="D34" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="J34" s="1" t="s">
+      <c r="H34" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L34" s="2"/>
-      <c r="N34" s="1" t="s">
+      <c r="L34" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="O34" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="1" t="s">
+      <c r="P34" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="15.75">
+      <c r="B35" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="F35" s="1" t="s">
+      <c r="D35" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="J35" s="1" t="s">
+      <c r="H35" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="L35" s="2"/>
-      <c r="N35" s="1" t="s">
+      <c r="L35" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="M35" s="1"/>
+      <c r="N35" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="O35" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
+      <c r="P35" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="15.75">
+      <c r="B36" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="F36" s="1" t="s">
+      <c r="D36" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="J36" s="1" t="s">
+      <c r="H36" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K36" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="L36" s="2"/>
-      <c r="N36" s="1" t="s">
+      <c r="L36" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M36" s="1"/>
+      <c r="N36" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="O36" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="P36" s="2"/>
+      <c r="P36" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>